<commit_message>
gráficos 2006 y 2008
</commit_message>
<xml_diff>
--- a/Congreso_2006/Datos_2006_filtrados.xlsx
+++ b/Congreso_2006/Datos_2006_filtrados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
   <si>
     <t xml:space="preserve">1. Nombres</t>
   </si>
@@ -1365,29 +1365,16 @@
   </si>
   <si>
     <t xml:space="preserve">Formación y educación en Hegel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NÚMEROS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Género</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ciudad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extranjero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1425,16 +1412,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1450,7 +1427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1463,13 +1440,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1498,7 +1468,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1519,19 +1489,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1554,13 +1512,13 @@
       <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF7E0021"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1582,648 +1540,44 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF83CAFF"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FFAECF00"/>
-      <rgbColor rgb="FFFFD320"/>
-      <rgbColor rgb="FFFF950E"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF004586"/>
-      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF314004"/>
+      <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF4B1F6F"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Proporción de género</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="1"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="1"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-            </c:dLbl>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="1"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$A$144:$A$145</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Femenino</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Masculino</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$B$144:$B$145</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>116</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Ciudades</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="314004"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="aecf00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4b1f6f"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff950e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$A$148:$A$157</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Bogotá</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Cali</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Barranquilla</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Bucaramanga</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Cartagena</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Manizales</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Medellín</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Pereira</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Tunja</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Extranjero</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$B$148:$B$157</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>18</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>158</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>466560</xdr:colOff>
-      <xdr:row>176</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="7067880"/>
-        <a:ext cx="5758560" cy="3232080"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>653400</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>6411960</xdr:colOff>
-      <xdr:row>162</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="5945400" y="4536360"/>
-        <a:ext cx="5758560" cy="3232080"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C144" activeCellId="0" sqref="C144"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2261,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -2284,7 +1638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>14</v>
       </c>
@@ -2307,7 +1661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>20</v>
       </c>
@@ -2353,7 +1707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>32</v>
       </c>
@@ -2376,7 +1730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>32</v>
       </c>
@@ -2399,7 +1753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>38</v>
       </c>
@@ -2422,7 +1776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>38</v>
       </c>
@@ -2445,7 +1799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>45</v>
       </c>
@@ -2468,7 +1822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>45</v>
       </c>
@@ -2514,7 +1868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>58</v>
       </c>
@@ -2537,7 +1891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>62</v>
       </c>
@@ -2560,7 +1914,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>66</v>
       </c>
@@ -2583,7 +1937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>72</v>
       </c>
@@ -2606,7 +1960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>77</v>
       </c>
@@ -2629,7 +1983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>80</v>
       </c>
@@ -2652,7 +2006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>83</v>
       </c>
@@ -2675,7 +2029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>88</v>
       </c>
@@ -2698,7 +2052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>91</v>
       </c>
@@ -2721,7 +2075,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>91</v>
       </c>
@@ -2781,7 +2135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>101</v>
       </c>
@@ -2804,7 +2158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>105</v>
       </c>
@@ -2827,7 +2181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>108</v>
       </c>
@@ -2850,7 +2204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>108</v>
       </c>
@@ -2873,7 +2227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>113</v>
       </c>
@@ -2896,7 +2250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>116</v>
       </c>
@@ -2919,7 +2273,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>118</v>
       </c>
@@ -2942,7 +2296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>122</v>
       </c>
@@ -2965,7 +2319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>127</v>
       </c>
@@ -2988,7 +2342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>129</v>
       </c>
@@ -3011,7 +2365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>132</v>
       </c>
@@ -3054,7 +2408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>139</v>
       </c>
@@ -3077,7 +2431,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>145</v>
       </c>
@@ -3100,7 +2454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>148</v>
       </c>
@@ -3123,7 +2477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>152</v>
       </c>
@@ -3189,7 +2543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>167</v>
       </c>
@@ -3235,7 +2589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>175</v>
       </c>
@@ -3258,7 +2612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>178</v>
       </c>
@@ -3281,7 +2635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>181</v>
       </c>
@@ -3304,7 +2658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>184</v>
       </c>
@@ -3327,7 +2681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>187</v>
       </c>
@@ -3350,7 +2704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>187</v>
       </c>
@@ -3393,7 +2747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>196</v>
       </c>
@@ -3416,7 +2770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>196</v>
       </c>
@@ -3439,7 +2793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>196</v>
       </c>
@@ -3462,7 +2816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>203</v>
       </c>
@@ -3485,7 +2839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>203</v>
       </c>
@@ -3508,7 +2862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>203</v>
       </c>
@@ -3531,7 +2885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>210</v>
       </c>
@@ -3574,7 +2928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>214</v>
       </c>
@@ -3597,7 +2951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>219</v>
       </c>
@@ -3620,7 +2974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>224</v>
       </c>
@@ -3643,7 +2997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>224</v>
       </c>
@@ -3666,7 +3020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>229</v>
       </c>
@@ -3689,7 +3043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>233</v>
       </c>
@@ -3712,7 +3066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>236</v>
       </c>
@@ -3732,7 +3086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>239</v>
       </c>
@@ -3755,7 +3109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>242</v>
       </c>
@@ -3778,7 +3132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>246</v>
       </c>
@@ -3801,7 +3155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>249</v>
       </c>
@@ -3870,7 +3224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>256</v>
       </c>
@@ -3890,7 +3244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>260</v>
       </c>
@@ -3913,7 +3267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>263</v>
       </c>
@@ -3936,7 +3290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>268</v>
       </c>
@@ -3959,7 +3313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>268</v>
       </c>
@@ -3982,7 +3336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>268</v>
       </c>
@@ -4005,7 +3359,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>274</v>
       </c>
@@ -4028,7 +3382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>277</v>
       </c>
@@ -4051,7 +3405,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>277</v>
       </c>
@@ -4074,7 +3428,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>282</v>
       </c>
@@ -4094,7 +3448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>286</v>
       </c>
@@ -4117,7 +3471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>289</v>
       </c>
@@ -4140,7 +3494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>289</v>
       </c>
@@ -4186,7 +3540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>298</v>
       </c>
@@ -4209,7 +3563,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>301</v>
       </c>
@@ -4232,7 +3586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>301</v>
       </c>
@@ -4255,7 +3609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>305</v>
       </c>
@@ -4278,7 +3632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>308</v>
       </c>
@@ -4301,7 +3655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
         <v>311</v>
       </c>
@@ -4324,7 +3678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>311</v>
       </c>
@@ -4347,7 +3701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>311</v>
       </c>
@@ -4370,7 +3724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>316</v>
       </c>
@@ -4393,7 +3747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>318</v>
       </c>
@@ -4416,7 +3770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>321</v>
       </c>
@@ -4439,7 +3793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>323</v>
       </c>
@@ -4462,7 +3816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>326</v>
       </c>
@@ -4485,7 +3839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>330</v>
       </c>
@@ -4508,7 +3862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>333</v>
       </c>
@@ -4528,7 +3882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>335</v>
       </c>
@@ -4551,7 +3905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>337</v>
       </c>
@@ -4574,7 +3928,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
         <v>340</v>
       </c>
@@ -4597,7 +3951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>340</v>
       </c>
@@ -4620,7 +3974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>340</v>
       </c>
@@ -4643,7 +3997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>346</v>
       </c>
@@ -4689,7 +4043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>348</v>
       </c>
@@ -4712,7 +4066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>354</v>
       </c>
@@ -4735,7 +4089,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>357</v>
       </c>
@@ -4758,7 +4112,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>361</v>
       </c>
@@ -4781,7 +4135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>364</v>
       </c>
@@ -4804,7 +4158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>368</v>
       </c>
@@ -4827,7 +4181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>371</v>
       </c>
@@ -4873,7 +4227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>374</v>
       </c>
@@ -4893,7 +4247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>374</v>
       </c>
@@ -4939,7 +4293,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>388</v>
       </c>
@@ -4962,7 +4316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>391</v>
       </c>
@@ -4985,7 +4339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>396</v>
       </c>
@@ -5005,7 +4359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>399</v>
       </c>
@@ -5028,7 +4382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>402</v>
       </c>
@@ -5051,7 +4405,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>405</v>
       </c>
@@ -5074,7 +4428,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>405</v>
       </c>
@@ -5097,7 +4451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>410</v>
       </c>
@@ -5120,7 +4474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>413</v>
       </c>
@@ -5143,7 +4497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>416</v>
       </c>
@@ -5166,7 +4520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>416</v>
       </c>
@@ -5258,7 +4612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>434</v>
       </c>
@@ -5281,7 +4635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>436</v>
       </c>
@@ -5304,7 +4658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>439</v>
       </c>
@@ -5327,7 +4681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>442</v>
       </c>
@@ -5350,7 +4704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>444</v>
       </c>
@@ -5374,131 +4728,40 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="4" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="B143" s="5"/>
-      <c r="C143" s="6"/>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B144" s="7" t="n">
-        <v>21</v>
-      </c>
-      <c r="C144" s="8"/>
-    </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B145" s="7" t="n">
-        <v>116</v>
-      </c>
-      <c r="C145" s="8"/>
+      <c r="B141" s="4"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="B147" s="5"/>
-      <c r="C147" s="6"/>
+      <c r="C147" s="5"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B148" s="7" t="n">
-        <v>75</v>
-      </c>
-      <c r="C148" s="6"/>
+      <c r="C148" s="5"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B149" s="7" t="n">
-        <v>12</v>
-      </c>
-      <c r="C149" s="6"/>
+      <c r="C149" s="5"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B150" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C150" s="6"/>
+      <c r="C150" s="5"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B151" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C151" s="6"/>
+      <c r="C151" s="5"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B152" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C152" s="6"/>
+      <c r="C152" s="5"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B153" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="C153" s="6"/>
+      <c r="C153" s="5"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B154" s="7" t="n">
-        <v>12</v>
-      </c>
-      <c r="C154" s="6"/>
+      <c r="C154" s="5"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="B155" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C155" s="6"/>
+      <c r="C155" s="5"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B156" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C156" s="6"/>
+      <c r="C156" s="5"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="B157" s="7" t="n">
-        <v>18</v>
-      </c>
-      <c r="C157" s="6"/>
+      <c r="C157" s="5"/>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D190" s="3"/>
@@ -5510,29 +4773,7 @@
       <c r="D199" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G138">
-    <filterColumn colId="5">
-      <filters>
-        <filter val=""/>
-        <filter val="Brasilia"/>
-        <filter val="Buenos Aires"/>
-        <filter val="Caracas"/>
-        <filter val="Humacao"/>
-        <filter val="Lima"/>
-        <filter val="London"/>
-        <filter val="México"/>
-        <filter val="Orlando (FLA)"/>
-        <filter val="Paris"/>
-        <filter val="Rio de Janeiro"/>
-        <filter val="Rosario"/>
-        <filter val="Toronto"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A147:B147"/>
-  </mergeCells>
+  <autoFilter ref="A1:G138"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
temas 2006. Progreso en datos 2016
</commit_message>
<xml_diff>
--- a/Congreso_2006/Datos_2006_filtrados.xlsx
+++ b/Congreso_2006/Datos_2006_filtrados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="447">
   <si>
     <t xml:space="preserve">1. Nombres</t>
   </si>
@@ -710,9 +710,6 @@
     <t xml:space="preserve">La metafísica de la participación en Agustín y Buenaventura</t>
   </si>
   <si>
-    <t xml:space="preserve">Coloquio Colombiano de Fenomenología</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hoover</t>
   </si>
   <si>
@@ -882,6 +879,9 @@
   </si>
   <si>
     <t xml:space="preserve">Apuntes filosóficos para una pedagogía afectiva: Levinas y la propuesta de la excepcionalidad desde la perspectiva de la filosofía del encuentro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educación</t>
   </si>
   <si>
     <t xml:space="preserve">Julián</t>
@@ -1577,7 +1577,7 @@
   <dimension ref="A1:G199"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D75" activeCellId="0" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3011,7 +3011,7 @@
         <v>227</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>228</v>
+        <v>65</v>
       </c>
       <c r="F63" s="0" t="s">
         <v>19</v>
@@ -3022,16 +3022,16 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B64" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="C64" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="D64" s="0" t="s">
         <v>231</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>232</v>
       </c>
       <c r="E64" s="0" t="s">
         <v>65</v>
@@ -3045,16 +3045,16 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B65" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>234</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>99</v>
@@ -3068,13 +3068,13 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="D66" s="0" t="s">
         <v>237</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>238</v>
       </c>
       <c r="E66" s="0" t="s">
         <v>76</v>
@@ -3088,16 +3088,16 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B67" s="0" t="s">
         <v>239</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>240</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>11</v>
@@ -3111,16 +3111,16 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B68" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="C68" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="D68" s="0" t="s">
         <v>244</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>245</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>18</v>
@@ -3134,16 +3134,16 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B69" s="0" t="s">
         <v>246</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>247</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E69" s="0" t="s">
         <v>208</v>
@@ -3157,16 +3157,16 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B70" s="0" t="s">
         <v>249</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>250</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>85</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E70" s="0" t="s">
         <v>87</v>
@@ -3180,16 +3180,16 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>30</v>
@@ -3203,16 +3203,16 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>28</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E72" s="0" t="s">
         <v>30</v>
@@ -3226,16 +3226,16 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B73" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="D73" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="E73" s="0" t="s">
         <v>258</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>259</v>
       </c>
       <c r="F73" s="0" t="s">
         <v>71</v>
@@ -3246,16 +3246,16 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B74" s="0" t="s">
         <v>260</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>261</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>41</v>
@@ -3269,19 +3269,19 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B75" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="C75" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="D75" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="E75" s="0" t="s">
         <v>266</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>267</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>19</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>200</v>
@@ -3301,7 +3301,7 @@
         <v>22</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>24</v>
@@ -3315,16 +3315,16 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>47</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>76</v>
@@ -3338,16 +3338,16 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E78" s="0" t="s">
         <v>76</v>
@@ -3361,16 +3361,16 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B79" s="0" t="s">
         <v>274</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>275</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E79" s="0" t="s">
         <v>65</v>
@@ -3384,16 +3384,16 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B80" s="0" t="s">
         <v>277</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>278</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E80" s="0" t="s">
         <v>65</v>
@@ -3407,16 +3407,16 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>103</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E81" s="0" t="s">
         <v>76</v>
@@ -3430,15 +3430,18 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B82" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="C82" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="D82" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="E82" s="0" t="s">
         <v>285</v>
       </c>
       <c r="F82" s="0" t="s">
@@ -3476,7 +3479,7 @@
         <v>289</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>68</v>
@@ -3571,7 +3574,7 @@
         <v>302</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>303</v>
@@ -3594,7 +3597,7 @@
         <v>302</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D89" s="0" t="s">
         <v>304</v>
@@ -3775,7 +3778,7 @@
         <v>321</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>68</v>
@@ -3887,7 +3890,7 @@
         <v>335</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>74</v>
@@ -3919,7 +3922,7 @@
         <v>339</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F103" s="0" t="s">
         <v>42</v>
@@ -3933,7 +3936,7 @@
         <v>340</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>74</v>
@@ -4002,7 +4005,7 @@
         <v>346</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>16</v>
@@ -4074,7 +4077,7 @@
         <v>355</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>356</v>
@@ -4367,7 +4370,7 @@
         <v>400</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>401</v>
@@ -4617,7 +4620,7 @@
         <v>434</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C134" s="0" t="s">
         <v>22</v>
@@ -4666,7 +4669,7 @@
         <v>440</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D136" s="0" t="s">
         <v>441</v>
@@ -4686,7 +4689,7 @@
         <v>442</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C137" s="0" t="s">
         <v>47</v>

</xml_diff>